<commit_message>
pandas file reading done
</commit_message>
<xml_diff>
--- a/MyPersonalData.xlsx
+++ b/MyPersonalData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fazlu\Working_space\class\Untitled Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fazlu\Working_space\class\python-Labraries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5772228F-0F0B-4322-AAAA-F891F5C9163C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DE92D7-788E-4284-8291-23B4C81AD849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{6CC6D833-2FBE-4CE7-98C9-C9DE09B91F94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6CC6D833-2FBE-4CE7-98C9-C9DE09B91F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>Searching</t>
   </si>
   <si>
-    <t>Revision</t>
-  </si>
-  <si>
     <t>Rough Idea</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>Daily Work</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -476,11 +476,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,6 +552,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,10 +867,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C583AD5-5703-48D1-B8D9-C2DEC9447A9D}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,9 +1128,17 @@
         <v>15</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
+        <v>16</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1872,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CF7744-FC5E-4645-8578-014A72B9EFF1}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2166,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="H18" s="27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
@@ -2156,9 +2176,7 @@
       <c r="B19" s="9"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="E19" s="11"/>
       <c r="F19" s="8"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
@@ -2175,10 +2193,10 @@
       <c r="D20" s="8"/>
       <c r="F20" s="8"/>
       <c r="H20" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2202,7 +2220,7 @@
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="H22" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I22" s="10"/>
     </row>
@@ -2216,7 +2234,7 @@
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="H23" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I23" s="10"/>
     </row>
@@ -2229,10 +2247,10 @@
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I24" s="10"/>
     </row>
@@ -2245,10 +2263,10 @@
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I25" s="10"/>
     </row>
@@ -2280,10 +2298,10 @@
         <v>44614</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>20</v>
@@ -2297,10 +2315,10 @@
         <v>44615</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>55</v>
@@ -2314,10 +2332,10 @@
         <v>44616</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>55</v>
@@ -2331,10 +2349,10 @@
         <v>44617</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>56</v>
@@ -2425,10 +2443,10 @@
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2442,10 +2460,10 @@
         <v>54</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2459,10 +2477,10 @@
         <v>54</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I39" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2476,10 +2494,10 @@
         <v>54</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I40" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2504,7 +2522,7 @@
         <v>54</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2516,7 +2534,7 @@
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2530,7 +2548,7 @@
         <v>54</v>
       </c>
       <c r="E44" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2544,7 +2562,7 @@
         <v>54</v>
       </c>
       <c r="E45" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2558,7 +2576,7 @@
         <v>54</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2572,7 +2590,7 @@
         <v>54</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2595,7 +2613,7 @@
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2609,7 +2627,7 @@
         <v>54</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2623,7 +2641,7 @@
         <v>54</v>
       </c>
       <c r="E51" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2637,7 +2655,7 @@
         <v>54</v>
       </c>
       <c r="E52" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2656,7 +2674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E2B70B-5504-4250-B4D9-D6A5107F0413}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2671,7 +2689,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2704,16 +2722,16 @@
         <v>42</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>